<commit_message>
Python DataCrawling_(Selenium Version 4 update Program)_22.08.30_AlphaVirsion_1.00_error check
</commit_message>
<xml_diff>
--- a/2.Python/WebCrawler/Excel/data/Crawling_data2.xlsx
+++ b/2.Python/WebCrawler/Excel/data/Crawling_data2.xlsx
@@ -1,40 +1,159 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="630" yWindow="570" windowWidth="12615" windowHeight="8100" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="630" yWindow="570" windowWidth="12615" windowHeight="8100"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
+  <si>
+    <t>업체명</t>
+  </si>
+  <si>
+    <t>주소</t>
+  </si>
+  <si>
+    <t>홈페이지</t>
+  </si>
+  <si>
+    <t>팩스번호</t>
+  </si>
+  <si>
+    <t>청록노인복지센터</t>
+  </si>
+  <si>
+    <t>부산 북구 만덕대로155번길 86-9 도개공아파트</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>실버타운청심빌리지</t>
+  </si>
+  <si>
+    <t>경기 가평군 설악면 미사리로 191-16</t>
+  </si>
+  <si>
+    <t>원불교하이원빌리지</t>
+  </si>
+  <si>
+    <t>서울 용산구 한강대로40가길 24 하이원빌리지</t>
+  </si>
+  <si>
+    <t>참사랑실버타운</t>
+  </si>
+  <si>
+    <t>대구 서구 가르뱅이로21길 3</t>
+  </si>
+  <si>
+    <t>한국노인복지진흥재단포천실버타운</t>
+  </si>
+  <si>
+    <t>경기 포천시 내촌면 금강로2536번길 112-12</t>
+  </si>
+  <si>
+    <t>늘푸른실버타운</t>
+  </si>
+  <si>
+    <t>대구 달성군 화원읍 명천로 331 금화복지재단 늘푸른실버타운</t>
+  </si>
+  <si>
+    <t>사회복지법인자혜복지재단노량실버타운</t>
+  </si>
+  <si>
+    <t>경남 하동군 금남면 연화마을길 49-15</t>
+  </si>
+  <si>
+    <t>https://blog.naver.com/silver-2011</t>
+  </si>
+  <si>
+    <t>예천실버요양원</t>
+  </si>
+  <si>
+    <t>경북 예천군 개포면 송담길 27-2</t>
+  </si>
+  <si>
+    <t>http://예천실버요양원.kr/</t>
+  </si>
+  <si>
+    <t>산청실버그룹홈</t>
+  </si>
+  <si>
+    <t>http://www.withangel.co.kr/</t>
+  </si>
+  <si>
+    <t>실버복지재단</t>
+  </si>
+  <si>
+    <t>경남 거창군 남하면 둔마리 산134-5</t>
+  </si>
+  <si>
+    <t>진명실버홈</t>
+  </si>
+  <si>
+    <t>대구 동구 동촌로 285 진명학원</t>
+  </si>
+  <si>
+    <t>http://www.jmsilver.or.kr/</t>
+  </si>
+  <si>
+    <t>대구광역시 동구 동촌로 285(방촌동 857-5번지) TEL . 053-985-8850 FAX. 053-984-8851
+COPYRIGHT (C) 2013 진명실버홈 ALL RIGHTS RESERVED.</t>
+  </si>
+  <si>
+    <t>대구샘노인요양센터</t>
+  </si>
+  <si>
+    <t>대구 달서구 진천로3길 80 1층</t>
+  </si>
+  <si>
+    <t>사회복지법인 보은복지재단</t>
+  </si>
+  <si>
+    <t>충북 보은군 내북면 남부로 6427-39</t>
+  </si>
+  <si>
+    <t>http://boeunbokji.modoo.at</t>
+  </si>
+  <si>
+    <t>아름다운요양원</t>
+  </si>
+  <si>
+    <t>대구 달성군 화원읍 명천로 331-1 금화복지재단 아름다운요양원</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
       <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
-      <family val="3"/>
-      <sz val="8"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -53,80 +172,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -414,23 +471,277 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="134.875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1"/>
-    <row r="2"/>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>